<commit_message>
séance 3 fini, supra
</commit_message>
<xml_diff>
--- a/data/data_cuivre_temp.xlsx
+++ b/data/data_cuivre_temp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Dev\Projets\phys_exp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E6D887-31D2-4652-B1D4-F0D9DEB203D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F8C5E78-5FFE-4A04-8800-C08126E82988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{7CFFD7A0-94A0-44FD-9881-2029062BD1C8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7CFFD7A0-94A0-44FD-9881-2029062BD1C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Température</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>AllResistivite</t>
+  </si>
+  <si>
+    <t>AllTemp</t>
   </si>
 </sst>
 </file>
@@ -411,7 +414,7 @@
   <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="104" zoomScaleNormal="104" workbookViewId="0">
-      <selection activeCell="H17" sqref="G15:H17"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -419,7 +422,7 @@
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.33203125" customWidth="1"/>
-    <col min="8" max="8" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
@@ -439,19 +442,22 @@
         <v>0</v>
       </c>
       <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2">
-        <f>F2-$F$2</f>
+        <f t="shared" ref="A2:A14" si="0">F2-$F$2</f>
         <v>0</v>
       </c>
       <c r="B2">
-        <f>C2*$O$8</f>
+        <f t="shared" ref="B2:B14" si="1">C2*$O$8</f>
         <v>9.4999999999999998E-3</v>
       </c>
       <c r="C2">
@@ -475,17 +481,21 @@
         <v>-22.4</v>
       </c>
       <c r="H2">
-        <f>$D$2*(1+0.0029*G2)</f>
-        <v>1.7441494094199814E-8</v>
+        <f>G2-22.4</f>
+        <v>-44.8</v>
+      </c>
+      <c r="I2">
+        <f>$D$2*(1+0.0029*H2)</f>
+        <v>1.622978180771023E-8</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3">
-        <f>F3-$F$2</f>
+        <f t="shared" si="0"/>
         <v>7.6000000000000014</v>
       </c>
       <c r="B3">
-        <f>C3*$O$8</f>
+        <f t="shared" si="1"/>
         <v>9.7000000000000003E-3</v>
       </c>
       <c r="C3">
@@ -493,7 +503,7 @@
         <v>97</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D14" si="0">(B3*PI()*(0.0005^2))/(4*0.1)</f>
+        <f t="shared" ref="D3:D14" si="2">(B3*PI()*(0.0005^2))/(4*0.1)</f>
         <v>1.9045905462388119E-8</v>
       </c>
       <c r="E3">
@@ -509,28 +519,32 @@
         <v>-12.399999999999999</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H15" si="1">$D$2*(1+0.0029*G3)</f>
-        <v>1.7982437079239805E-8</v>
+        <f t="shared" ref="H3:H14" si="3">G3-22.4</f>
+        <v>-34.799999999999997</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I14" si="4">$D$2*(1+0.0029*H3)</f>
+        <v>1.6770724792750222E-8</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4">
-        <f>F4-$F$2</f>
+        <f t="shared" si="0"/>
         <v>12.600000000000001</v>
       </c>
       <c r="B4">
-        <f>C4*$O$8</f>
+        <f t="shared" si="1"/>
         <v>9.9000000000000008E-3</v>
       </c>
       <c r="C4">
         <v>99</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.9438604544086845E-8</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E14" si="2">B4/$B$2-1</f>
+        <f t="shared" ref="E4:E14" si="5">B4/$B$2-1</f>
         <v>4.2105263157894868E-2</v>
       </c>
       <c r="F4">
@@ -538,21 +552,25 @@
         <v>35</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:G15" si="3">G3+10</f>
+        <f t="shared" ref="G4:G13" si="6">G3+10</f>
         <v>-2.3999999999999986</v>
       </c>
       <c r="H4">
-        <f t="shared" si="1"/>
-        <v>1.85233800642798E-8</v>
+        <f t="shared" si="3"/>
+        <v>-24.799999999999997</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="4"/>
+        <v>1.7311667777790217E-8</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5">
-        <f>F5-$F$2</f>
+        <f t="shared" si="0"/>
         <v>17.600000000000001</v>
       </c>
       <c r="B5">
-        <f>C5*$O$8</f>
+        <f t="shared" si="1"/>
         <v>0.01</v>
       </c>
       <c r="C5">
@@ -560,11 +578,11 @@
         <v>100</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.9634954084936204E-8</v>
       </c>
       <c r="E5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>5.2631578947368363E-2</v>
       </c>
       <c r="F5">
@@ -572,21 +590,25 @@
         <v>40</v>
       </c>
       <c r="G5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>7.6000000000000014</v>
       </c>
       <c r="H5">
-        <f t="shared" si="1"/>
-        <v>1.9064323049319792E-8</v>
+        <f t="shared" si="3"/>
+        <v>-14.799999999999997</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="4"/>
+        <v>1.7852610762830209E-8</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6">
-        <f>F6-$F$2</f>
+        <f t="shared" si="0"/>
         <v>22.6</v>
       </c>
       <c r="B6">
-        <f>C6*$O$8</f>
+        <f t="shared" si="1"/>
         <v>1.0100000000000001E-2</v>
       </c>
       <c r="C6">
@@ -594,11 +616,11 @@
         <v>101</v>
       </c>
       <c r="D6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.9831303625785567E-8</v>
       </c>
       <c r="E6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6.3157894736842302E-2</v>
       </c>
       <c r="F6">
@@ -606,21 +628,25 @@
         <v>45</v>
       </c>
       <c r="G6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>17.600000000000001</v>
       </c>
       <c r="H6">
-        <f t="shared" si="1"/>
-        <v>1.9605266034359784E-8</v>
+        <f t="shared" si="3"/>
+        <v>-4.7999999999999972</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="4"/>
+        <v>1.83935537478702E-8</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7">
-        <f>F7-$F$2</f>
+        <f t="shared" si="0"/>
         <v>27.6</v>
       </c>
       <c r="B7">
-        <f>C7*$O$8</f>
+        <f t="shared" si="1"/>
         <v>1.0200000000000001E-2</v>
       </c>
       <c r="C7">
@@ -628,11 +654,11 @@
         <v>102</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.0027653166634933E-8</v>
       </c>
       <c r="E7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>7.3684210526315796E-2</v>
       </c>
       <c r="F7">
@@ -640,21 +666,25 @@
         <v>50</v>
       </c>
       <c r="G7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>27.6</v>
       </c>
       <c r="H7">
-        <f t="shared" si="1"/>
-        <v>2.0146209019399775E-8</v>
+        <f t="shared" si="3"/>
+        <v>5.2000000000000028</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="4"/>
+        <v>1.8934496732910192E-8</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8">
-        <f>F8-$F$2</f>
+        <f t="shared" si="0"/>
         <v>32.6</v>
       </c>
       <c r="B8">
-        <f>C8*$O$8</f>
+        <f t="shared" si="1"/>
         <v>1.0400000000000001E-2</v>
       </c>
       <c r="C8">
@@ -662,11 +692,11 @@
         <v>104</v>
       </c>
       <c r="D8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.0420352248333655E-8</v>
       </c>
       <c r="E8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>9.473684210526323E-2</v>
       </c>
       <c r="F8">
@@ -674,12 +704,16 @@
         <v>55</v>
       </c>
       <c r="G8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>37.6</v>
       </c>
       <c r="H8">
-        <f t="shared" si="1"/>
-        <v>2.068715200443977E-8</v>
+        <f t="shared" si="3"/>
+        <v>15.200000000000003</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="4"/>
+        <v>1.9475439717950187E-8</v>
       </c>
       <c r="O8">
         <f>10^-4</f>
@@ -688,11 +722,11 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9">
-        <f>F9-$F$2</f>
+        <f t="shared" si="0"/>
         <v>37.6</v>
       </c>
       <c r="B9">
-        <f>C9*$O$8</f>
+        <f t="shared" si="1"/>
         <v>1.0500000000000001E-2</v>
       </c>
       <c r="C9">
@@ -700,11 +734,11 @@
         <v>105</v>
       </c>
       <c r="D9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.0616701789183015E-8</v>
       </c>
       <c r="E9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.10526315789473695</v>
       </c>
       <c r="F9">
@@ -712,21 +746,25 @@
         <v>60</v>
       </c>
       <c r="G9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>47.6</v>
       </c>
       <c r="H9">
-        <f t="shared" si="1"/>
-        <v>2.1228094989479762E-8</v>
+        <f t="shared" si="3"/>
+        <v>25.200000000000003</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="4"/>
+        <v>2.0016382702990178E-8</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10">
-        <f>F10-$F$2</f>
+        <f t="shared" si="0"/>
         <v>42.6</v>
       </c>
       <c r="B10">
-        <f>C10*$O$8</f>
+        <f t="shared" si="1"/>
         <v>1.06E-2</v>
       </c>
       <c r="C10">
@@ -734,11 +772,11 @@
         <v>106</v>
       </c>
       <c r="D10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.0813051330032381E-8</v>
       </c>
       <c r="E10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.11578947368421066</v>
       </c>
       <c r="F10">
@@ -746,21 +784,25 @@
         <v>65</v>
       </c>
       <c r="G10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>57.6</v>
       </c>
       <c r="H10">
-        <f t="shared" si="1"/>
-        <v>2.1769037974519757E-8</v>
+        <f t="shared" si="3"/>
+        <v>35.200000000000003</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="4"/>
+        <v>2.055732568803017E-8</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11">
-        <f>F11-$F$2</f>
+        <f t="shared" si="0"/>
         <v>47.6</v>
       </c>
       <c r="B11">
-        <f>C11*$O$8</f>
+        <f t="shared" si="1"/>
         <v>1.0800000000000001E-2</v>
       </c>
       <c r="C11">
@@ -768,11 +810,11 @@
         <v>108</v>
       </c>
       <c r="D11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.1205750411731103E-8</v>
       </c>
       <c r="E11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.13684210526315788</v>
       </c>
       <c r="F11">
@@ -780,21 +822,25 @@
         <v>70</v>
       </c>
       <c r="G11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>67.599999999999994</v>
       </c>
       <c r="H11">
-        <f t="shared" si="1"/>
-        <v>2.2309980959559745E-8</v>
+        <f t="shared" si="3"/>
+        <v>45.199999999999996</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="4"/>
+        <v>2.1098268673070162E-8</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12">
-        <f>F12-$F$2</f>
+        <f t="shared" si="0"/>
         <v>52.6</v>
       </c>
       <c r="B12">
-        <f>C12*$O$8</f>
+        <f t="shared" si="1"/>
         <v>1.09E-2</v>
       </c>
       <c r="C12">
@@ -802,11 +848,11 @@
         <v>109</v>
       </c>
       <c r="D12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.1402099952580463E-8</v>
       </c>
       <c r="E12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.14736842105263159</v>
       </c>
       <c r="F12">
@@ -814,21 +860,25 @@
         <v>75</v>
       </c>
       <c r="G12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>77.599999999999994</v>
       </c>
       <c r="H12">
-        <f t="shared" si="1"/>
-        <v>2.2850923944599737E-8</v>
+        <f t="shared" si="3"/>
+        <v>55.199999999999996</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="4"/>
+        <v>2.1639211658110157E-8</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13">
-        <f>F13-$F$2</f>
+        <f t="shared" si="0"/>
         <v>57.6</v>
       </c>
       <c r="B13">
-        <f>C13*$O$8</f>
+        <f t="shared" si="1"/>
         <v>1.11E-2</v>
       </c>
       <c r="C13">
@@ -836,11 +886,11 @@
         <v>111</v>
       </c>
       <c r="D13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.1794799034279191E-8</v>
       </c>
       <c r="E13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.16842105263157903</v>
       </c>
       <c r="F13">
@@ -848,21 +898,25 @@
         <v>80</v>
       </c>
       <c r="G13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>87.6</v>
       </c>
       <c r="H13">
-        <f t="shared" si="1"/>
-        <v>2.3391866929639732E-8</v>
+        <f t="shared" si="3"/>
+        <v>65.199999999999989</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="4"/>
+        <v>2.2180154643150145E-8</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14">
-        <f>F14-$F$2</f>
+        <f t="shared" si="0"/>
         <v>62.6</v>
       </c>
       <c r="B14">
-        <f>C14*$O$8</f>
+        <f t="shared" si="1"/>
         <v>1.1300000000000001E-2</v>
       </c>
       <c r="C14">
@@ -870,11 +924,11 @@
         <v>113</v>
       </c>
       <c r="D14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.2187498115977914E-8</v>
       </c>
       <c r="E14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.18947368421052646</v>
       </c>
       <c r="F14">
@@ -886,8 +940,12 @@
         <v>97.6</v>
       </c>
       <c r="H14">
-        <f t="shared" si="1"/>
-        <v>2.3932809914679723E-8</v>
+        <f t="shared" si="3"/>
+        <v>75.199999999999989</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="4"/>
+        <v>2.2721097628190143E-8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>